<commit_message>
Grouping database generation into one script
</commit_message>
<xml_diff>
--- a/Inputs/ARES_Africa/Fuel_Prices.xlsx
+++ b/Inputs/ARES_Africa/Fuel_Prices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\Inputs\ARES_Africa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0872D9F0-FD65-4AEF-9B3E-5400A4F3C119}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECBEA57-99C0-4291-8BCD-EE7FF348C113}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CAA3788-42FB-4D90-BFA9-C8BAE54B809C}"/>
+    <workbookView xWindow="18885" yWindow="5955" windowWidth="18900" windowHeight="11055" xr2:uid="{6CAA3788-42FB-4D90-BFA9-C8BAE54B809C}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -35,18 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
   <si>
     <t>Coastal</t>
   </si>
   <si>
     <t>Inland</t>
-  </si>
-  <si>
-    <t>OIL</t>
-  </si>
-  <si>
-    <t>GAS</t>
   </si>
   <si>
     <t>HRD</t>
@@ -570,159 +564,223 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330942BE-0393-411D-B067-329244D2C7F3}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="2">
+        <f>B3*0.9</f>
+        <v>26.811</v>
+      </c>
+      <c r="C2" s="2">
+        <f t="shared" ref="C2:D2" si="0">C3*0.9</f>
+        <v>34.757999999999996</v>
+      </c>
+      <c r="D2" s="2">
+        <f t="shared" si="0"/>
+        <v>47.988</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="2">
+        <v>29.79</v>
+      </c>
+      <c r="C3" s="2">
+        <v>38.619999999999997</v>
+      </c>
+      <c r="D3" s="2">
+        <v>53.32</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="2">
+        <f>B3*1.1</f>
+        <v>32.768999999999998</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:D4" si="1">C3*1.1</f>
+        <v>42.481999999999999</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="1"/>
+        <v>58.652000000000008</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="2">
+        <f>B6*0.9</f>
+        <v>17.595000000000002</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" ref="C5:E5" si="2">C6*0.9</f>
+        <v>22.715999999999998</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="2"/>
+        <v>30.168000000000003</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="2"/>
+        <v>39.609000000000002</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>51</v>
       </c>
-      <c r="B2">
-        <v>7.04</v>
-      </c>
-      <c r="C2" s="2">
-        <v>9.7777777777777786</v>
-      </c>
-      <c r="D2" s="2">
-        <v>11.932203389830509</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="C3" s="2">
-        <v>11.527777777777779</v>
-      </c>
-      <c r="D3" s="2">
-        <v>14.067796610169493</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4">
-        <v>9.2100000000000009</v>
-      </c>
-      <c r="C4" s="2">
-        <v>12.791666666666668</v>
-      </c>
-      <c r="D4" s="2">
-        <v>15.610169491525426</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" s="2">
+        <v>19.55</v>
+      </c>
+      <c r="C6" s="2">
+        <v>25.24</v>
+      </c>
+      <c r="D6" s="2">
+        <v>33.520000000000003</v>
+      </c>
+      <c r="E6" s="2">
+        <v>44.01</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>52</v>
       </c>
-      <c r="B5">
-        <v>5.42</v>
-      </c>
-      <c r="C5">
-        <v>6.9443749999999991</v>
-      </c>
-      <c r="D5">
-        <v>7.5371874999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" s="2">
+        <f>B6*1.1</f>
+        <v>21.505000000000003</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:E7" si="3">C6*1.1</f>
+        <v>27.763999999999999</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="3"/>
+        <v>36.872000000000007</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="3"/>
+        <v>48.411000000000001</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>53</v>
       </c>
-      <c r="B6">
-        <v>5.75</v>
-      </c>
-      <c r="C6">
-        <v>6.9676470588235286</v>
-      </c>
-      <c r="D6">
-        <v>7.4411764705882364</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
+        <v>75</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>54</v>
       </c>
-      <c r="B7">
-        <v>6.01</v>
-      </c>
-      <c r="C7">
-        <v>7.0305660377358494</v>
-      </c>
-      <c r="D7">
-        <v>7.4274528301886784</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2">
+        <v>80</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>55</v>
       </c>
-      <c r="D8">
-        <v>2.9154266211604094</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9">
-        <v>3.3911262798634811</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10">
-        <v>3.7710580204778159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
+        <v>90</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11">
-        <v>2.9</v>
-      </c>
-      <c r="F11">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2">
+        <v>10.08</v>
+      </c>
+      <c r="G11" s="2">
+        <v>30.24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12">
-        <v>2.6</v>
-      </c>
-      <c r="F12">
-        <v>7.8</v>
+        <v>4</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2">
+        <v>9.36</v>
+      </c>
+      <c r="G12" s="2">
+        <v>28.08</v>
       </c>
     </row>
   </sheetData>
@@ -738,7 +796,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,45 +825,45 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
         <v>43</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>44</v>
-      </c>
-      <c r="M1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -858,7 +916,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -911,7 +969,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -964,7 +1022,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1017,7 +1075,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1070,7 +1128,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1123,7 +1181,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1176,7 +1234,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1229,7 +1287,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1282,7 +1340,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1335,7 +1393,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1388,7 +1446,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1441,7 +1499,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1494,7 +1552,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1547,7 +1605,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1600,7 +1658,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1653,7 +1711,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1706,7 +1764,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1726,14 +1784,14 @@
         <v>1</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -1759,7 +1817,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1812,7 +1870,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1832,14 +1890,14 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -1865,7 +1923,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1885,14 +1943,14 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -1918,7 +1976,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1970,7 +2028,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2023,7 +2081,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2076,7 +2134,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -2146,372 +2204,216 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A199DECB-9A5D-45DD-B99A-020513F48653}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B4">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B3">
-        <v>1440</v>
-      </c>
-      <c r="C3">
-        <v>1070</v>
-      </c>
-      <c r="D3">
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="B5">
         <v>1427</v>
       </c>
-      <c r="C5">
-        <v>322</v>
-      </c>
-      <c r="D5">
-        <v>1427</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="B12">
         <v>324</v>
       </c>
-      <c r="C12">
-        <v>324</v>
-      </c>
-      <c r="D12">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="B19">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19">
-        <v>1500</v>
-      </c>
-      <c r="C19">
-        <v>855</v>
-      </c>
-      <c r="D19">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="B22">
         <v>1617</v>
       </c>
-      <c r="C22">
-        <v>439</v>
-      </c>
-      <c r="D22">
-        <v>1617</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B23">
-        <v>1464</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>1464</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="B26">
-        <v>1146</v>
-      </c>
-      <c r="C26">
-        <v>317</v>
-      </c>
-      <c r="D26">
         <v>1146</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Database for the whole African continent
</commit_message>
<xml_diff>
--- a/Inputs/ARES_Africa/Fuel_Prices.xlsx
+++ b/Inputs/ARES_Africa/Fuel_Prices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\Inputs\ARES_Africa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECBEA57-99C0-4291-8BCD-EE7FF348C113}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCCB4A5-2BCF-44E4-ADBB-93EB316B0622}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18885" yWindow="5955" windowWidth="18900" windowHeight="11055" xr2:uid="{6CAA3788-42FB-4D90-BFA9-C8BAE54B809C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CAA3788-42FB-4D90-BFA9-C8BAE54B809C}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="80">
   <si>
     <t>Coastal</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Inland</t>
   </si>
   <si>
-    <t>HRD</t>
-  </si>
-  <si>
     <t>BIO</t>
   </si>
   <si>
@@ -203,6 +200,81 @@
   </si>
   <si>
     <t>Hrd - Max</t>
+  </si>
+  <si>
+    <t>BJ</t>
+  </si>
+  <si>
+    <t>BW</t>
+  </si>
+  <si>
+    <t>BF</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>GH</t>
+  </si>
+  <si>
+    <t>GN</t>
+  </si>
+  <si>
+    <t>GW</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>MZ</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>ZA</t>
+  </si>
+  <si>
+    <t>SZ</t>
+  </si>
+  <si>
+    <t>TG</t>
+  </si>
+  <si>
+    <t>ZM</t>
+  </si>
+  <si>
+    <t>ZW</t>
+  </si>
+  <si>
+    <t>Rail</t>
+  </si>
+  <si>
+    <t>Road</t>
   </si>
 </sst>
 </file>
@@ -244,12 +316,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,34 +642,34 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2">
         <f>B3*0.9</f>
@@ -614,7 +689,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2">
         <v>29.79</v>
@@ -631,7 +706,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2">
         <f>B3*1.1</f>
@@ -651,7 +726,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2">
         <f>B6*0.9</f>
@@ -674,7 +749,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="2">
         <v>19.55</v>
@@ -693,7 +768,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="2">
         <f>B6*1.1</f>
@@ -716,9 +791,11 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="B8" s="2">
+        <v>70</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2">
         <v>75</v>
@@ -729,9 +806,11 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="B9" s="2">
+        <v>75</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2">
         <v>80</v>
@@ -742,9 +821,11 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>54</v>
+      </c>
+      <c r="B10" s="2">
+        <v>85</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2">
         <v>90</v>
@@ -755,7 +836,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -770,7 +851,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -790,13 +871,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF816D95-8BFE-4C2C-8200-EF0F84B8458E}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,45 +906,45 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>40</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>41</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
         <v>42</v>
       </c>
-      <c r="M1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>43</v>
-      </c>
-      <c r="O1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -879,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F22" si="0">1-D2</f>
+        <f t="shared" ref="F2:F49" si="0">IF(OR(D2=1,E2=1),0,1)</f>
         <v>0</v>
       </c>
       <c r="G2">
@@ -889,7 +970,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <f>IF(OR(G2=1,H2=1),0,1)</f>
+        <f t="shared" ref="I2:I49" si="1">IF(OR(G2=1,H2=1),0,1)</f>
         <v>0</v>
       </c>
       <c r="J2">
@@ -903,26 +984,25 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <f>1-L2</f>
+        <f t="shared" ref="M2:M49" si="2">1-L2</f>
         <v>0</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2">
-        <f>1-N2</f>
+        <f t="shared" ref="O2:O49" si="3">1-N2</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C26" si="1">1-B3</f>
         <v>1</v>
       </c>
       <c r="D3">
@@ -942,147 +1022,145 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I26" si="2">IF(OR(G3=1,H3=1),0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K26" si="3">1-J3</f>
+        <f t="shared" ref="K3:K5" si="4">1-J3</f>
         <v>1</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M26" si="4">1-L3</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O26" si="5">1-N3</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="C4:C49" si="5">1-B4</f>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
+      <c r="A6" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1095,46 +1173,46 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" ref="K6:K49" si="6">1-J6</f>
+        <v>0</v>
       </c>
       <c r="L6">
         <v>1</v>
       </c>
       <c r="M6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D7">
@@ -1148,47 +1226,47 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>1</v>
       </c>
       <c r="M7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1207,40 +1285,40 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N8">
         <v>0</v>
       </c>
       <c r="O8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D9">
@@ -1254,53 +1332,52 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
@@ -1310,54 +1387,54 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N10">
         <v>0</v>
       </c>
       <c r="O10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1366,41 +1443,41 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1419,47 +1496,47 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
@@ -1469,50 +1546,50 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="N13">
         <v>0</v>
       </c>
       <c r="O13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
@@ -1522,43 +1599,43 @@
         <v>1</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D15">
@@ -1578,146 +1655,146 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L15">
         <v>1</v>
       </c>
       <c r="M15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N16">
         <v>0</v>
       </c>
       <c r="O16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
       <c r="K17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D18">
@@ -1731,47 +1808,47 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="J18">
         <v>0</v>
       </c>
       <c r="K18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N18">
         <v>0</v>
       </c>
       <c r="O18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1784,57 +1861,57 @@
         <v>1</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="J19">
         <v>0</v>
       </c>
       <c r="K19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="N19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O19">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1843,40 +1920,40 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J20">
         <v>0</v>
       </c>
       <c r="K20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N20">
         <v>0</v>
       </c>
       <c r="O20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D21">
@@ -1896,51 +1973,51 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N21">
         <v>0</v>
       </c>
       <c r="O21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1949,50 +2026,51 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J22">
         <v>0</v>
       </c>
       <c r="K22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N22">
         <v>0</v>
       </c>
       <c r="O22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -2001,193 +2079,1426 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
-        <f>1-D24</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="J24">
         <v>0</v>
       </c>
       <c r="K24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N24">
         <v>0</v>
       </c>
       <c r="O24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <f>1-D25</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="J25">
         <v>0</v>
       </c>
       <c r="K25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N25">
         <v>0</v>
       </c>
       <c r="O25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26">
-        <f>1-D26</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="J26">
         <v>0</v>
       </c>
       <c r="K26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="N26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:O26">
-    <cfRule type="colorScale" priority="2">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Q2:Q69">
+    <sortCondition ref="Q2"/>
+  </sortState>
+  <conditionalFormatting sqref="G2:L2 B2:E49 G5:H49 I7:N7 I8:K49 I5:J5 G3:J4 K3:L5 O2:O46 L8:N46 I6:L6 M2:N6 L47:O49">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F49">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2204,217 +3515,548 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A199DECB-9A5D-45DD-B99A-020513F48653}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3">
+        <v>715</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B4">
+        <v>1228</v>
+      </c>
+      <c r="C4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6">
+        <v>852</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
-        <v>1508</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B7">
+        <v>360</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B8">
+        <v>772</v>
+      </c>
+      <c r="C8">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
-        <v>1427</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B16">
+        <v>324</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25">
+        <v>366</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28">
+        <v>743</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30">
+        <v>455</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33">
+        <v>681</v>
+      </c>
+      <c r="C33">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B35">
+        <v>1401</v>
+      </c>
+      <c r="C35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19">
-        <v>1464</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="B40">
+        <v>1331</v>
+      </c>
+      <c r="C40">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41">
+        <v>182</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B22">
-        <v>1617</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B42">
+        <v>772</v>
+      </c>
+      <c r="C42">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B23">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26">
-        <v>1146</v>
+      <c r="B46">
+        <v>1060</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48">
+        <v>935</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49">
+        <v>182</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>